<commit_message>
1. Changed the response keys of category and subcategory to category_id and subcategory_id; 2. Refactor the data structure of JSONHelper and SQLHelper from List to Map; 3. Built the data schema for 'Comment' table.
</commit_message>
<xml_diff>
--- a/doc/PostgreSQL_Data_Dictionary.xlsx
+++ b/doc/PostgreSQL_Data_Dictionary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="137">
   <si>
     <t>user 用户表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -257,14 +257,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>read_by_reply</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>read_by_activity_holder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cid</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -381,19 +373,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>reply_to</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>user_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>aid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -730,10 +714,10 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1079,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12:N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -1095,22 +1079,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:14" ht="18" customHeight="1">
-      <c r="B3" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="I3" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
+      <c r="B3" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="I3" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
     </row>
     <row r="4" spans="2:14" ht="18" customHeight="1">
       <c r="B4" s="1" t="s">
@@ -1157,14 +1141,14 @@
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="I5" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>47</v>
@@ -1183,14 +1167,14 @@
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="I6" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>41</v>
@@ -1206,19 +1190,19 @@
     </row>
     <row r="7" spans="2:14" ht="18" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="I7" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>41</v>
@@ -1234,13 +1218,13 @@
     </row>
     <row r="8" spans="2:14" ht="18" customHeight="1">
       <c r="B8" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -1260,10 +1244,10 @@
     </row>
     <row r="9" spans="2:14" ht="18" customHeight="1">
       <c r="B9" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>15</v>
@@ -1288,10 +1272,10 @@
     </row>
     <row r="10" spans="2:14" ht="18" customHeight="1">
       <c r="B10" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>18</v>
@@ -1299,27 +1283,13 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="I10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="11" spans="2:14" ht="18" customHeight="1">
       <c r="B11" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>15</v>
@@ -1327,48 +1297,58 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="I11" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
     </row>
     <row r="12" spans="2:14" ht="18" customHeight="1">
-      <c r="I12" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3" t="b">
+      <c r="I12" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="2:14" ht="18" customHeight="1">
+      <c r="I13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="18" customHeight="1">
+      <c r="B14" s="8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:14" ht="18" customHeight="1">
-      <c r="B14" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="I14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
     </row>
     <row r="15" spans="2:14" ht="18" customHeight="1">
       <c r="B15" s="1" t="s">
@@ -1389,48 +1369,46 @@
       <c r="G15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
+      <c r="I15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
     </row>
     <row r="16" spans="2:14" ht="18" customHeight="1">
       <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D16" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="I16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="I16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
     </row>
     <row r="17" spans="2:14" ht="18" customHeight="1">
       <c r="B17" s="3" t="s">
@@ -1439,19 +1417,19 @@
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="3" t="s">
         <v>61</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>9</v>
       </c>
       <c r="L17" s="3"/>
@@ -1465,7 +1443,7 @@
       <c r="C18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="3"/>
@@ -1473,18 +1451,6 @@
         <v>18</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="I18" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
     </row>
     <row r="19" spans="2:14" ht="18" customHeight="1">
       <c r="B19" s="3" t="s">
@@ -1493,26 +1459,14 @@
       <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>94</v>
+      <c r="D19" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
     </row>
     <row r="20" spans="2:14" ht="18" customHeight="1">
       <c r="B20" s="3" t="s">
@@ -1527,25 +1481,21 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="I20" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
+      <c r="I20" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
     </row>
     <row r="21" spans="2:14" ht="18" customHeight="1">
       <c r="B21" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>18</v>
@@ -1553,13 +1503,31 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
+      <c r="I21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" spans="2:14" ht="18" customHeight="1">
       <c r="B22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>23</v>
@@ -1567,114 +1535,92 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
+      <c r="I22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
     </row>
     <row r="23" spans="2:14" ht="18" customHeight="1">
       <c r="B23" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
+        <v>92</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
     </row>
     <row r="24" spans="2:14" ht="18" customHeight="1">
       <c r="B24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" ht="18" customHeight="1">
-      <c r="I25" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-    </row>
-    <row r="26" spans="2:14" ht="18" customHeight="1">
-      <c r="I26" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
+      <c r="I24" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
     </row>
     <row r="27" spans="2:14" ht="18" customHeight="1">
-      <c r="B27" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="I27" s="3" t="s">
+      <c r="B27" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="I27" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="J27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
     </row>
     <row r="28" spans="2:14" ht="18" customHeight="1">
       <c r="B28" s="1" t="s">
@@ -1695,6 +1641,24 @@
       <c r="G28" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="29" spans="2:14" ht="18" customHeight="1">
       <c r="B29" s="2" t="s">
@@ -1703,12 +1667,24 @@
       <c r="C29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
+      <c r="I29" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
     </row>
     <row r="30" spans="2:14" ht="18" customHeight="1">
       <c r="B30" s="3" t="s">
@@ -1717,20 +1693,24 @@
       <c r="C30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="I30" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
+      <c r="I30" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
     </row>
     <row r="31" spans="2:14" ht="18" customHeight="1">
       <c r="B31" s="3" t="s">
@@ -1739,30 +1719,24 @@
       <c r="C31" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>128</v>
+      <c r="D31" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="I31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="I31" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
     </row>
     <row r="32" spans="2:14" ht="18" customHeight="1">
       <c r="B32" s="3" t="s">
@@ -1771,22 +1745,24 @@
       <c r="C32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>128</v>
+      <c r="D32" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-      <c r="I32" s="2" t="s">
+      <c r="I32" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J32" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="J32" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="K32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L32" s="3"/>
+      <c r="L32" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
     </row>
@@ -1797,7 +1773,7 @@
       <c r="C33" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>34</v>
       </c>
       <c r="E33" s="3"/>
@@ -1805,81 +1781,51 @@
       <c r="G33" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I33" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
     </row>
     <row r="34" spans="2:14" ht="18" customHeight="1">
       <c r="B34" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>85</v>
+      <c r="D34" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
-      <c r="I34" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
     </row>
     <row r="35" spans="2:14" ht="18" customHeight="1">
       <c r="B35" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
-      <c r="I35" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L35" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
+      <c r="I35" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
     </row>
     <row r="36" spans="2:14" ht="18" customHeight="1">
       <c r="B36" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="7" t="s">
         <v>38</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -1887,20 +1833,52 @@
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
+      <c r="I36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="37" spans="2:14" ht="18" customHeight="1">
       <c r="B37" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
+      <c r="I37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
     </row>
     <row r="38" spans="2:14" ht="18" customHeight="1">
       <c r="B38" s="4" t="s">
@@ -1909,56 +1887,54 @@
       <c r="C38" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="7" t="s">
         <v>42</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
-      <c r="I38" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
+      <c r="I38" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K38" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
     </row>
     <row r="39" spans="2:14" ht="18" customHeight="1">
       <c r="B39" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="I39" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N39" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="I39" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
     </row>
     <row r="40" spans="2:14" ht="18" customHeight="1">
       <c r="B40" s="3" t="s">
@@ -1968,55 +1944,55 @@
         <v>41</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3">
         <v>0</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="I40" s="3" t="s">
         <v>74</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="K40" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L40" s="3" t="s">
-        <v>73</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
     </row>
     <row r="41" spans="2:14" ht="18" customHeight="1">
       <c r="B41" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3">
         <v>0</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>82</v>
+      <c r="I41" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K41" s="8" t="s">
-        <v>84</v>
+        <v>76</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
+      <c r="N41" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="2:14" ht="18" customHeight="1">
       <c r="B42" s="3" t="s">
@@ -2025,7 +2001,7 @@
       <c r="C42" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="7" t="s">
         <v>46</v>
       </c>
       <c r="E42" s="3"/>
@@ -2033,72 +2009,32 @@
       <c r="G42" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I42" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K42" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
     </row>
     <row r="43" spans="2:14" ht="18" customHeight="1">
       <c r="B43" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>94</v>
+        <v>104</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
-      <c r="I43" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J43" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-    </row>
-    <row r="44" spans="2:14" ht="18" customHeight="1">
-      <c r="I44" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="J44" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="K44" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="46" spans="2:14" ht="18" customHeight="1">
-      <c r="B46" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
+      <c r="B46" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
     </row>
     <row r="47" spans="2:14" ht="18" customHeight="1">
       <c r="B47" s="1" t="s">
@@ -2122,7 +2058,7 @@
     </row>
     <row r="48" spans="2:14" ht="18" customHeight="1">
       <c r="B48" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>8</v>
@@ -2152,7 +2088,7 @@
     </row>
     <row r="50" spans="2:7" ht="18" customHeight="1">
       <c r="B50" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>41</v>
@@ -2167,14 +2103,14 @@
       <c r="G50" s="3"/>
     </row>
     <row r="53" spans="2:7" ht="18" customHeight="1">
-      <c r="B53" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
+      <c r="B53" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
     </row>
     <row r="54" spans="2:7" ht="18" customHeight="1">
       <c r="B54" s="1" t="s">
@@ -2198,7 +2134,7 @@
     </row>
     <row r="55" spans="2:7" ht="18" customHeight="1">
       <c r="B55" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>8</v>
@@ -2228,7 +2164,7 @@
     </row>
     <row r="57" spans="2:7" ht="18" customHeight="1">
       <c r="B57" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>41</v>
@@ -2244,16 +2180,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="I12:N12"/>
+    <mergeCell ref="I20:N20"/>
+    <mergeCell ref="I27:N27"/>
+    <mergeCell ref="B3:G3"/>
     <mergeCell ref="B46:G46"/>
     <mergeCell ref="B53:G53"/>
-    <mergeCell ref="I38:N38"/>
+    <mergeCell ref="I35:N35"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="B27:G27"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="I15:N15"/>
-    <mergeCell ref="I23:N23"/>
-    <mergeCell ref="I30:N30"/>
-    <mergeCell ref="B3:G3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>